<commit_message>
Add a notas en DDBB V1
</commit_message>
<xml_diff>
--- a/DDBB_V1.xlsx
+++ b/DDBB_V1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodro\Dropbox\ICM-Compartido\Modelación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\Documents\GitHub\Prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171DBD81-7B28-4A93-B1AE-8EE1FCDDD2D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986ED31C-E11A-4280-B8FF-C1687CAAE1C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" activeTab="8" xr2:uid="{274CBEC6-4746-4300-96A8-6383DBCE5EFB}"/>
+    <workbookView xWindow="28692" yWindow="-108" windowWidth="29016" windowHeight="16416" activeTab="2" xr2:uid="{274CBEC6-4746-4300-96A8-6383DBCE5EFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="126">
   <si>
     <t>Red Existente</t>
   </si>
@@ -445,6 +445,12 @@
   </si>
   <si>
     <t>ESQ</t>
+  </si>
+  <si>
+    <t>Notas de desarrollo a futuro</t>
+  </si>
+  <si>
+    <t>Idealmente, desde esta BD se generará un archivo para cada modelo con las características necesarias</t>
   </si>
 </sst>
 </file>
@@ -710,35 +716,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -753,6 +732,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1130,16 +1136,18 @@
   </sheetPr>
   <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1150,13 +1158,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
       <c r="C3" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1164,13 +1172,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1178,35 +1186,35 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="25"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
+      <c r="C13" s="31"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="25"/>
+      <c r="C15" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1235,7 +1243,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1246,23 +1254,32 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B1:B2"/>
+  <dimension ref="B1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="84.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1282,23 +1299,23 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="19"/>
-    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" style="19"/>
+    <col min="2" max="2" width="42.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
@@ -1307,7 +1324,7 @@
       </c>
       <c r="C2" s="21"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>18</v>
       </c>
@@ -1319,7 +1336,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>19</v>
       </c>
@@ -1331,7 +1348,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>123</v>
       </c>
@@ -1343,7 +1360,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>61</v>
       </c>
@@ -1352,7 +1369,7 @@
       </c>
       <c r="C6" s="21"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>34</v>
       </c>
@@ -1361,7 +1378,7 @@
       </c>
       <c r="C7" s="21"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>36</v>
       </c>
@@ -1370,7 +1387,7 @@
       </c>
       <c r="C8" s="21"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>122</v>
       </c>
@@ -1379,7 +1396,7 @@
       </c>
       <c r="C9" s="21"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>59</v>
       </c>
@@ -1390,7 +1407,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>63</v>
       </c>
@@ -1401,7 +1418,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>89</v>
       </c>
@@ -1412,7 +1429,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>67</v>
       </c>
@@ -1423,7 +1440,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>98</v>
       </c>
@@ -1434,7 +1451,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>109</v>
       </c>
@@ -1445,7 +1462,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>86</v>
       </c>
@@ -1456,7 +1473,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>70</v>
       </c>
@@ -1467,7 +1484,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>73</v>
       </c>
@@ -1478,7 +1495,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>78</v>
       </c>
@@ -1489,7 +1506,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>79</v>
       </c>
@@ -1500,7 +1517,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>96</v>
       </c>
@@ -1511,7 +1528,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>81</v>
       </c>
@@ -1522,7 +1539,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>82</v>
       </c>
@@ -1533,7 +1550,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>91</v>
       </c>
@@ -1544,7 +1561,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
         <v>94</v>
       </c>
@@ -1555,7 +1572,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
         <v>101</v>
       </c>
@@ -1566,7 +1583,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>105</v>
       </c>
@@ -1577,7 +1594,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
         <v>106</v>
       </c>
@@ -1588,7 +1605,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
         <v>111</v>
       </c>
@@ -1596,7 +1613,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>113</v>
       </c>
@@ -1607,7 +1624,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
         <v>116</v>
       </c>
@@ -1618,7 +1635,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>119</v>
       </c>
@@ -1649,40 +1666,40 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.44140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>15</v>
       </c>
@@ -1774,7 +1791,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1796,7 +1813,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1811,7 +1828,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1826,7 +1843,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1839,48 +1856,48 @@
   </sheetPr>
   <dimension ref="A1:AE18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" style="14" customWidth="1"/>
-    <col min="7" max="7" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="35.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:31" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38"/>
       <c r="G1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="33"/>
-    </row>
-    <row r="3" spans="1:31" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35"/>
+    </row>
+    <row r="3" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -1892,10 +1909,10 @@
       <c r="D3" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="36"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="13" t="s">
         <v>19</v>
       </c>
@@ -1908,71 +1925,71 @@
       <c r="J3" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="30" t="s">
+      <c r="K3" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="30" t="s">
+      <c r="L3" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="M3" s="30" t="s">
+      <c r="M3" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="N3" s="30" t="s">
+      <c r="N3" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="O3" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="Q3" s="30" t="s">
+      <c r="Q3" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="R3" s="30" t="s">
+      <c r="R3" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="S3" s="30" t="s">
+      <c r="S3" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="T3" s="30" t="s">
+      <c r="T3" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="U3" s="30" t="s">
+      <c r="U3" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="V3" s="30" t="s">
+      <c r="V3" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="W3" s="30" t="s">
+      <c r="W3" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="X3" s="30" t="s">
+      <c r="X3" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="Y3" s="30" t="s">
+      <c r="Y3" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="Z3" s="30" t="s">
+      <c r="Z3" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="AA3" s="30" t="s">
+      <c r="AA3" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="AB3" s="30" t="s">
+      <c r="AB3" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="AC3" s="30" t="s">
+      <c r="AC3" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="AD3" s="30" t="s">
+      <c r="AD3" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="AE3" s="30" t="s">
+      <c r="AE3" s="24" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2016,7 +2033,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="G5" t="s">
         <v>40</v>
       </c>
@@ -2045,7 +2062,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
         <v>41</v>
       </c>
@@ -2074,7 +2091,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F7" s="17"/>
       <c r="G7" s="16" t="s">
         <v>42</v>
@@ -2104,7 +2121,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2138,7 +2155,7 @@
       <c r="L8">
         <v>12</v>
       </c>
-      <c r="M8" s="38">
+      <c r="M8" s="29">
         <v>0</v>
       </c>
       <c r="N8">
@@ -2148,7 +2165,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
         <v>46</v>
       </c>
@@ -2167,7 +2184,7 @@
       <c r="L9">
         <v>12</v>
       </c>
-      <c r="M9" s="38">
+      <c r="M9" s="29">
         <v>0</v>
       </c>
       <c r="N9">
@@ -2177,7 +2194,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="G10" t="s">
         <v>47</v>
       </c>
@@ -2206,7 +2223,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="G11" t="s">
         <v>48</v>
       </c>
@@ -2235,7 +2252,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="G12" t="s">
         <v>49</v>
       </c>
@@ -2264,7 +2281,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="G13" t="s">
         <v>50</v>
       </c>
@@ -2293,7 +2310,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F14" s="17"/>
       <c r="G14" s="16" t="s">
         <v>51</v>
@@ -2323,7 +2340,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2357,7 +2374,7 @@
       <c r="L15">
         <v>12</v>
       </c>
-      <c r="M15" s="38">
+      <c r="M15" s="29">
         <v>0</v>
       </c>
       <c r="N15">
@@ -2367,7 +2384,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="G16" t="s">
         <v>53</v>
       </c>
@@ -2396,7 +2413,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:15" x14ac:dyDescent="0.3">
       <c r="G17" t="s">
         <v>54</v>
       </c>
@@ -2425,7 +2442,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="6:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:15" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F18" s="17"/>
       <c r="G18" s="16" t="s">
         <v>55</v>

</xml_diff>